<commit_message>
Created new table (survival-data) for analysis on survival rates by vials
</commit_message>
<xml_diff>
--- a/data/raw_data.xlsx
+++ b/data/raw_data.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/day/Documents/Year 2/Summer Project/Project/FLY/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85595595-A679-9649-B6DD-C0D78ACA6798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46E7C68-9AE8-0641-9D22-1643D4DCB355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="1080" windowWidth="18800" windowHeight="16540" activeTab="2" xr2:uid="{BFC1D339-3DB5-C448-B6A9-500BCE707C03}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16900" activeTab="4" xr2:uid="{BFC1D339-3DB5-C448-B6A9-500BCE707C03}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch2" sheetId="2" r:id="rId1"/>
     <sheet name="Batch3" sheetId="1" r:id="rId2"/>
     <sheet name="Batch4" sheetId="3" r:id="rId3"/>
     <sheet name="Batch5" sheetId="5" r:id="rId4"/>
+    <sheet name="Batch6" sheetId="6" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="msg.Eng">[1]RES!$B$59</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="127">
   <si>
     <t>25 degrees constant, egg laid: 8/7 11:00</t>
   </si>
@@ -345,6 +346,90 @@
   <si>
     <t>2025-08-11 15:00:00 BST</t>
   </si>
+  <si>
+    <t>25 degrees constant, egg laid: 11/8 11:00</t>
+  </si>
+  <si>
+    <t>25 degrees constant, egg laid: 12/8 11:00</t>
+  </si>
+  <si>
+    <t>O6</t>
+  </si>
+  <si>
+    <t>2025-08-19 11:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-19 13:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-19 15:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-19 17:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-20 11:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-20 13:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-20 15:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-20 17:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-21 11:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-21 13:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-21 15:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-21 17:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-22 11:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-22 13:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-22 15:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-22 17:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-23 11:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-23 13:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-23 15:00:00 BST</t>
+  </si>
+  <si>
+    <t>2025-08-23 17:00:00 BST</t>
+  </si>
+  <si>
+    <t>25 degrees low fluctuation, egg laid: 11/8 11:00</t>
+  </si>
+  <si>
+    <t>25 degrees high fluctuation, egg laid: 11/8 11:00</t>
+  </si>
+  <si>
+    <t>2025-08-12 11:00:00 BST</t>
+  </si>
+  <si>
+    <t>25 degrees low fluctuation, egg laid: 12/8 11:00</t>
+  </si>
+  <si>
+    <t>25 degrees high fluctuation, egg laid: 12/8 11:00</t>
+  </si>
 </sst>
 </file>
 
@@ -366,12 +451,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="19">
@@ -602,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -630,6 +721,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4227,8 +4324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F991F7-8DB8-7441-B265-C993206F1DF9}">
   <dimension ref="A1:V81"/>
   <sheetViews>
-    <sheetView topLeftCell="B32" zoomScale="50" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81:V81"/>
+    <sheetView zoomScale="50" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9364,8 +9461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506B60B4-DC64-6843-B110-BA2E7C354F8F}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76:K76"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11880,12 +11977,3599 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F62D36-AFDA-4442-8035-A7F3425CB3C0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A30" zoomScale="66" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:S72"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="5"/>
+    </row>
+    <row r="2" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+    </row>
+    <row r="6" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+    </row>
+    <row r="10" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+    </row>
+    <row r="14" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+    </row>
+    <row r="18" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+    </row>
+    <row r="22" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S26" s="5"/>
+    </row>
+    <row r="27" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O27" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q27" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="R27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="S27" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+    </row>
+    <row r="31" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+    </row>
+    <row r="35" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+    </row>
+    <row r="39" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A40" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A42" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+    </row>
+    <row r="43" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A44" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A45" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
+      <c r="S45" s="16"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A46" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+    </row>
+    <row r="47" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S51" s="5"/>
+    </row>
+    <row r="52" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H52" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L52" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M52" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O52" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P52" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q52" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="R52" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="S52" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="16"/>
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A55" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+    </row>
+    <row r="56" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="8"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="18"/>
+      <c r="Q57" s="18"/>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16"/>
+      <c r="M58" s="16"/>
+      <c r="N58" s="16"/>
+      <c r="O58" s="16"/>
+      <c r="P58" s="16"/>
+      <c r="Q58" s="16"/>
+      <c r="R58" s="16"/>
+      <c r="S58" s="16"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A59" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="16"/>
+      <c r="N59" s="16"/>
+      <c r="O59" s="16"/>
+      <c r="P59" s="16"/>
+      <c r="Q59" s="16"/>
+      <c r="R59" s="16"/>
+      <c r="S59" s="16"/>
+    </row>
+    <row r="60" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8"/>
+      <c r="O60" s="8"/>
+      <c r="P60" s="8"/>
+      <c r="Q60" s="8"/>
+      <c r="R60" s="8"/>
+      <c r="S60" s="8"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A61" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="18"/>
+      <c r="Q61" s="18"/>
+      <c r="R61" s="18"/>
+      <c r="S61" s="18"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A62" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="16"/>
+      <c r="L62" s="16"/>
+      <c r="M62" s="16"/>
+      <c r="N62" s="16"/>
+      <c r="O62" s="16"/>
+      <c r="P62" s="16"/>
+      <c r="Q62" s="16"/>
+      <c r="R62" s="16"/>
+      <c r="S62" s="16"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A63" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="16"/>
+      <c r="M63" s="16"/>
+      <c r="N63" s="16"/>
+      <c r="O63" s="16"/>
+      <c r="P63" s="16"/>
+      <c r="Q63" s="16"/>
+      <c r="R63" s="16"/>
+      <c r="S63" s="16"/>
+    </row>
+    <row r="64" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="8"/>
+      <c r="M64" s="8"/>
+      <c r="N64" s="8"/>
+      <c r="O64" s="8"/>
+      <c r="P64" s="8"/>
+      <c r="Q64" s="8"/>
+      <c r="R64" s="8"/>
+      <c r="S64" s="8"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A65" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+      <c r="M65" s="18"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="18"/>
+      <c r="P65" s="18"/>
+      <c r="Q65" s="18"/>
+      <c r="R65" s="18"/>
+      <c r="S65" s="18"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A66" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66" s="16"/>
+      <c r="M66" s="16"/>
+      <c r="N66" s="16"/>
+      <c r="O66" s="16"/>
+      <c r="P66" s="16"/>
+      <c r="Q66" s="16"/>
+      <c r="R66" s="16"/>
+      <c r="S66" s="16"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A67" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="16"/>
+      <c r="N67" s="16"/>
+      <c r="O67" s="16"/>
+      <c r="P67" s="16"/>
+      <c r="Q67" s="16"/>
+      <c r="R67" s="16"/>
+      <c r="S67" s="16"/>
+    </row>
+    <row r="68" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="8"/>
+      <c r="N68" s="8"/>
+      <c r="O68" s="8"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="8"/>
+      <c r="R68" s="8"/>
+      <c r="S68" s="8"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A69" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B69" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="18"/>
+      <c r="M69" s="18"/>
+      <c r="N69" s="18"/>
+      <c r="O69" s="18"/>
+      <c r="P69" s="18"/>
+      <c r="Q69" s="18"/>
+      <c r="R69" s="18"/>
+      <c r="S69" s="18"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A70" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+      <c r="J70" s="16"/>
+      <c r="K70" s="16"/>
+      <c r="L70" s="16"/>
+      <c r="M70" s="16"/>
+      <c r="N70" s="16"/>
+      <c r="O70" s="16"/>
+      <c r="P70" s="16"/>
+      <c r="Q70" s="16"/>
+      <c r="R70" s="16"/>
+      <c r="S70" s="16"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A71" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="16"/>
+      <c r="L71" s="16"/>
+      <c r="M71" s="16"/>
+      <c r="N71" s="16"/>
+      <c r="O71" s="16"/>
+      <c r="P71" s="16"/>
+      <c r="Q71" s="16"/>
+      <c r="R71" s="16"/>
+      <c r="S71" s="16"/>
+    </row>
+    <row r="72" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B72" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="8"/>
+      <c r="P72" s="8"/>
+      <c r="Q72" s="8"/>
+      <c r="R72" s="8"/>
+      <c r="S72" s="8"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A73" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A905B976-4036-4E44-976D-CCAD2EDD0D32}">
+  <dimension ref="A1:S73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:S72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="5"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+    </row>
+    <row r="6" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+    </row>
+    <row r="10" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+    </row>
+    <row r="14" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+    </row>
+    <row r="18" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+    </row>
+    <row r="22" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q23" s="29"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S26" s="5"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P27" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q27" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="R27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="S27" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+    </row>
+    <row r="31" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+    </row>
+    <row r="35" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+    </row>
+    <row r="39" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A40" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A42" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+    </row>
+    <row r="43" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A44" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A45" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
+      <c r="S45" s="16"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A46" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+    </row>
+    <row r="47" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S51" s="5"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L52" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M52" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N52" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O52" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P52" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q52" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="R52" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="S52" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="16"/>
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A55" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+    </row>
+    <row r="56" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="8"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="18"/>
+      <c r="Q57" s="18"/>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16"/>
+      <c r="M58" s="16"/>
+      <c r="N58" s="16"/>
+      <c r="O58" s="16"/>
+      <c r="P58" s="16"/>
+      <c r="Q58" s="16"/>
+      <c r="R58" s="16"/>
+      <c r="S58" s="16"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A59" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="16"/>
+      <c r="N59" s="16"/>
+      <c r="O59" s="16"/>
+      <c r="P59" s="16"/>
+      <c r="Q59" s="16"/>
+      <c r="R59" s="16"/>
+      <c r="S59" s="16"/>
+    </row>
+    <row r="60" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8"/>
+      <c r="O60" s="8"/>
+      <c r="P60" s="8"/>
+      <c r="Q60" s="8"/>
+      <c r="R60" s="8"/>
+      <c r="S60" s="8"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A61" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="18"/>
+      <c r="Q61" s="18"/>
+      <c r="R61" s="18"/>
+      <c r="S61" s="18"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A62" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="16"/>
+      <c r="L62" s="16"/>
+      <c r="M62" s="16"/>
+      <c r="N62" s="16"/>
+      <c r="O62" s="16"/>
+      <c r="P62" s="16"/>
+      <c r="Q62" s="16"/>
+      <c r="R62" s="16"/>
+      <c r="S62" s="16"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A63" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="16"/>
+      <c r="M63" s="16"/>
+      <c r="N63" s="16"/>
+      <c r="O63" s="16"/>
+      <c r="P63" s="16"/>
+      <c r="Q63" s="16"/>
+      <c r="R63" s="16"/>
+      <c r="S63" s="16"/>
+    </row>
+    <row r="64" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="8"/>
+      <c r="M64" s="8"/>
+      <c r="N64" s="8"/>
+      <c r="O64" s="8"/>
+      <c r="P64" s="8"/>
+      <c r="Q64" s="8"/>
+      <c r="R64" s="8"/>
+      <c r="S64" s="8"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A65" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+      <c r="M65" s="18"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="18"/>
+      <c r="P65" s="18"/>
+      <c r="Q65" s="18"/>
+      <c r="R65" s="18"/>
+      <c r="S65" s="18"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A66" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66" s="16"/>
+      <c r="M66" s="16"/>
+      <c r="N66" s="16"/>
+      <c r="O66" s="16"/>
+      <c r="P66" s="16"/>
+      <c r="Q66" s="16"/>
+      <c r="R66" s="16"/>
+      <c r="S66" s="16"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A67" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="16"/>
+      <c r="N67" s="16"/>
+      <c r="O67" s="16"/>
+      <c r="P67" s="16"/>
+      <c r="Q67" s="16"/>
+      <c r="R67" s="16"/>
+      <c r="S67" s="16"/>
+    </row>
+    <row r="68" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="8"/>
+      <c r="N68" s="8"/>
+      <c r="O68" s="8"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="8"/>
+      <c r="R68" s="8"/>
+      <c r="S68" s="8"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A69" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B69" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="18"/>
+      <c r="M69" s="18"/>
+      <c r="N69" s="18"/>
+      <c r="O69" s="18"/>
+      <c r="P69" s="18"/>
+      <c r="Q69" s="18"/>
+      <c r="R69" s="18"/>
+      <c r="S69" s="18"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A70" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B70" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+      <c r="J70" s="16"/>
+      <c r="K70" s="16"/>
+      <c r="L70" s="16"/>
+      <c r="M70" s="16"/>
+      <c r="N70" s="16"/>
+      <c r="O70" s="16"/>
+      <c r="P70" s="16"/>
+      <c r="Q70" s="16"/>
+      <c r="R70" s="16"/>
+      <c r="S70" s="16"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A71" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="16"/>
+      <c r="L71" s="16"/>
+      <c r="M71" s="16"/>
+      <c r="N71" s="16"/>
+      <c r="O71" s="16"/>
+      <c r="P71" s="16"/>
+      <c r="Q71" s="16"/>
+      <c r="R71" s="16"/>
+      <c r="S71" s="16"/>
+    </row>
+    <row r="72" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B72" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="8"/>
+      <c r="P72" s="8"/>
+      <c r="Q72" s="8"/>
+      <c r="R72" s="8"/>
+      <c r="S72" s="8"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A73" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>